<commit_message>
add user context in interface
</commit_message>
<xml_diff>
--- a/input/part1.xlsx
+++ b/input/part1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyProjects\company-description\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6C91CF-BF4D-40A0-8E48-8D72598039D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD329F37-8DE9-43AC-A772-AA258DE06E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23016" yWindow="-96" windowWidth="23016" windowHeight="12336" xr2:uid="{36112B11-FB1C-42E5-9462-4C8EEC29C988}"/>
+    <workbookView xWindow="-23040" yWindow="-396" windowWidth="23016" windowHeight="12336" xr2:uid="{36112B11-FB1C-42E5-9462-4C8EEC29C988}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>CBS</t>
-  </si>
-  <si>
-    <t>CBS News</t>
   </si>
   <si>
     <t>CBS Studios International</t>
   </si>
   <si>
     <t>Cellnex</t>
-  </si>
-  <si>
-    <t>Ceska Televize (Czech Television)</t>
-  </si>
-  <si>
-    <t>Ceske Radiokomunikace (CRa)</t>
-  </si>
-  <si>
-    <t>Cetin</t>
-  </si>
-  <si>
-    <t>Channel 4 (UK)</t>
   </si>
 </sst>
 </file>
@@ -431,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3238CE47-101B-4088-9E03-2C955D1305B6}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A100"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,37 +431,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>